<commit_message>
remove ADM Type from varible definitions
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.3_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.3_PH2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Variables</t>
   </si>
@@ -22,9 +22,6 @@
     <t>ADM Name</t>
   </si>
   <si>
-    <t>ADM Type</t>
-  </si>
-  <si>
     <t>PID</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>The name of the ADM that was run against the multi-kdma target</t>
   </si>
   <si>
-    <t>The type of ADM (baseline or aligned) that was run against the multi-kdma target</t>
-  </si>
-  <si>
     <t>The Participant ID used to generate the MJ and IO alignment targets.</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
   </si>
   <si>
     <t>Levels</t>
-  </si>
-  <si>
-    <t>baseline or aligned</t>
   </si>
   <si>
     <t>phase1-adept-eval-MJ2, 	phase1-adept-eval-MJ4, 	phase1-adept-eval-MJ5, DryRunEval-MJ2-eval, DryRunEval-MJ4-eval, DryRunEval-MJ5-eval</t>
@@ -243,7 +234,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,12 +245,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -291,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -299,17 +284,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,47 +589,46 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="4" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="4" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="4" width="40.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="4" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="3" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="3" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="3" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="3" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="3" width="40.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="3" width="32.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,7 +638,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -693,25 +668,25 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -729,314 +704,302 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="159" customFormat="1" s="1">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="133.5" customFormat="1" s="1">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="159" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Itm 946 baseline multikdma (#279)
* started adding baseline data to multikdma table

* updated variable definitions

* revert selectedEval change

* remove ADM Type from varible definitions
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.3_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ2.3_PH2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Variables</t>
   </si>
@@ -22,9 +22,6 @@
     <t>ADM Name</t>
   </si>
   <si>
-    <t>ADM Type</t>
-  </si>
-  <si>
     <t>PID</t>
   </si>
   <si>
@@ -40,40 +37,76 @@
     <t>IO Alignment Target</t>
   </si>
   <si>
-    <t>MJ KDMA - MJ2</t>
-  </si>
-  <si>
-    <t>MJ KDMA - MJ4</t>
-  </si>
-  <si>
-    <t>MJ KDMA - MJ5</t>
-  </si>
-  <si>
-    <t>MJ KDMA - AVE</t>
-  </si>
-  <si>
-    <t>IO KDMA - MJ2</t>
-  </si>
-  <si>
-    <t>IO KDMA - MJ4</t>
-  </si>
-  <si>
-    <t>IO KDMA - MJ5</t>
-  </si>
-  <si>
-    <t>IO KDMA - AVE</t>
-  </si>
-  <si>
-    <t>Alignment (Target|ADM_MJ2)</t>
-  </si>
-  <si>
-    <t>Alignment (Target|ADM_MJ4)</t>
-  </si>
-  <si>
-    <t>Alignment (Target|ADM_MJ5)</t>
-  </si>
-  <si>
-    <t>Alignment Average (Target|ADM)</t>
+    <t>MJ KDMA_Aligned - MJ2</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Aligned - MJ4</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Aligned - MJ5</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Aligned - AVE</t>
+  </si>
+  <si>
+    <t>IO KDMA_Aligned - MJ2</t>
+  </si>
+  <si>
+    <t>IO KDMA_Aligned - MJ4</t>
+  </si>
+  <si>
+    <t>IO KDMA_Aligned - MJ5</t>
+  </si>
+  <si>
+    <t>IO KDMA_Aligned - AVE</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ2)_Aligned</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ4)_Aligned</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ5)_Aligned</t>
+  </si>
+  <si>
+    <t>Alignment Average (Target|ADM)_Aligned</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Baseline - MJ2</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Baseline - MJ4</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Baseline - MJ5</t>
+  </si>
+  <si>
+    <t>MJ KDMA_Baseline - AVE</t>
+  </si>
+  <si>
+    <t>IO KDMA_Baseline - MJ2</t>
+  </si>
+  <si>
+    <t>IO KDMA_Baseline - MJ4</t>
+  </si>
+  <si>
+    <t>IO KDMA_Baseline - MJ5</t>
+  </si>
+  <si>
+    <t>IO KDMA_Baseline - AVE</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ2)_Baseline</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ4)_Baseline</t>
+  </si>
+  <si>
+    <t>Alignment (Target|ADM_MJ5)_Baseline</t>
+  </si>
+  <si>
+    <t>Alignment Average (Target|ADM)_Baseline</t>
   </si>
   <si>
     <t>Source</t>
@@ -97,9 +130,6 @@
     <t>The name of the ADM that was run against the multi-kdma target</t>
   </si>
   <si>
-    <t>The type of ADM (baseline or aligned) that was run against the multi-kdma target</t>
-  </si>
-  <si>
     <t>The Participant ID used to generate the MJ and IO alignment targets.</t>
   </si>
   <si>
@@ -115,46 +145,79 @@
     <t>The Ingroup Bias KDMA value that the ADM is expected to align to, based on the human scenario output</t>
   </si>
   <si>
-    <t>The ADM's Moral Judgement KDMA when aligning to the target at the MJ2 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The ADM's Moral Judgement KDMA when aligning to the target at the MJ4 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The ADM's Moral Judgement KDMA when aligning to the target at the MJ5 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The average of the ADM's Moral Judgement KDMAs</t>
-  </si>
-  <si>
-    <t>The ADM's Ingroup Bias KDMA when aligning to the target at the MJ2 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The ADM's Ingroup Bias KDMA when aligning to the target at the MJ4 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The ADM's Ingroup Bias KDMA when aligning to the target at the MJ5 evaluation scenario</t>
-  </si>
-  <si>
-    <t>The average of the ADM's Ingroup Bias KDMAs</t>
-  </si>
-  <si>
-    <t>The alignment between the human whose KDMAs generated the alignment target and the ADM's probe responses for MJ2</t>
-  </si>
-  <si>
-    <t>The alignment between the human whose KDMAs generated the alignment target and the ADM's probe responses for MJ4</t>
-  </si>
-  <si>
-    <t>The alignment between the human whose KDMAs generated the alignment target and the ADM's probe responses for MJ5</t>
-  </si>
-  <si>
-    <t>The average of all 3 alignment scores between the human and ADM</t>
+    <t>The aligned ADM's Moral Judgement KDMA when aligning to the target at the MJ2 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The aligned ADM's Moral Judgement KDMA when aligning to the target at the MJ4 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The aligned ADM's Moral Judgement KDMA when aligning to the target at the MJ5 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The average of the aligned ADM's Moral Judgement KDMAs</t>
+  </si>
+  <si>
+    <t>The aligned ADM's Ingroup Bias KDMA when aligning to the target at the MJ2 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The aligned ADM's Ingroup Bias KDMA when aligning to the target at the MJ4 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The aligned ADM's Ingroup Bias KDMA when aligning to the target at the MJ5 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The average of the aligned ADM's Ingroup Bias KDMAs</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the aligned ADM's probe responses for MJ2</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the aligned ADM's probe responses for MJ4</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the aligned ADM's probe responses for MJ5</t>
+  </si>
+  <si>
+    <t>The average of all 3 alignment scores between the human and aligned ADM</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Moral Judgement KDMA when aligning to the target at the MJ2 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Moral Judgement KDMA when aligning to the target at the MJ4 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Moral Judgement KDMA when aligning to the target at the MJ5 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The average of the baseline ADM's Moral Judgement KDMAs</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Ingroup Bias KDMA when aligning to the target at the MJ2 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Ingroup Bias KDMA when aligning to the target at the MJ4 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The baseline ADM's Ingroup Bias KDMA when aligning to the target at the MJ5 evaluation scenario</t>
+  </si>
+  <si>
+    <t>The average of the baseline ADM's Ingroup Bias KDMAs</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the baseline ADM's probe responses for MJ2</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the baseline ADM's probe responses for MJ4</t>
+  </si>
+  <si>
+    <t>The alignment between the human whose KDMAs generated the alignment target and the baseline ADM's probe responses for MJ5</t>
+  </si>
+  <si>
+    <t>The average of all 3 alignment scores between the human and baseline ADM</t>
   </si>
   <si>
     <t>Levels</t>
-  </si>
-  <si>
-    <t>baseline or aligned</t>
   </si>
   <si>
     <t>phase1-adept-eval-MJ2, 	phase1-adept-eval-MJ4, 	phase1-adept-eval-MJ5, DryRunEval-MJ2-eval, DryRunEval-MJ4-eval, DryRunEval-MJ5-eval</t>
@@ -181,7 +244,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -213,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -222,13 +285,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,35 +589,46 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="4" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="4" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="4" width="40.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="4" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="3" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="3" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="3" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="3" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="3" width="40.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="3" width="32.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="57" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +638,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -600,206 +668,338 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="126" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="159" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="150" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="159" customFormat="1" s="1">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>